<commit_message>
I forgot what I've added
</commit_message>
<xml_diff>
--- a/uploads/Testing.xlsx
+++ b/uploads/Testing.xlsx
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="14">
   <si>
     <t xml:space="preserve">lrn</t>
   </si>
   <si>
-    <t xml:space="preserve">firstName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">middleName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastName</t>
+    <t xml:space="preserve">fullName</t>
   </si>
   <si>
     <t xml:space="preserve">gradeLevel</t>
@@ -43,49 +37,28 @@
     <t xml:space="preserve">Abdul</t>
   </si>
   <si>
-    <t xml:space="preserve">Salani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kribek</t>
-  </si>
-  <si>
     <t xml:space="preserve">Section B</t>
   </si>
   <si>
     <t xml:space="preserve">Clementine</t>
   </si>
   <si>
-    <t xml:space="preserve">Roses</t>
-  </si>
-  <si>
     <t xml:space="preserve">Secion Y</t>
   </si>
   <si>
     <t xml:space="preserve">Bill</t>
   </si>
   <si>
-    <t xml:space="preserve">Gates</t>
-  </si>
-  <si>
     <t xml:space="preserve">Section W</t>
   </si>
   <si>
     <t xml:space="preserve">Steve</t>
   </si>
   <si>
-    <t xml:space="preserve">Jobs</t>
-  </si>
-  <si>
     <t xml:space="preserve">Section A</t>
   </si>
   <si>
     <t xml:space="preserve">Linus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tips</t>
   </si>
   <si>
     <t xml:space="preserve">Section C</t>
@@ -185,10 +158,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -210,31 +183,19 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>106167030444</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,16 +203,13 @@
         <v>103243766545</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="0" t="n">
         <v>7</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,16 +217,13 @@
         <v>106672080991</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>7</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,36 +231,209 @@
         <v>113344505123</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>101010111001</v>
+        <v>108327392163</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>119329323003</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>145327323922</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>177564264669</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>103213211651</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>132344665123</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>101665701001</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>113344990867</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>132326739001</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>113827008323</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>106567776651</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>104534367001</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>183276482643</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>137275574891</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FileType Checking on Upload
</commit_message>
<xml_diff>
--- a/uploads/Testing.xlsx
+++ b/uploads/Testing.xlsx
@@ -406,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Served the index page
</commit_message>
<xml_diff>
--- a/uploads/Testing.xlsx
+++ b/uploads/Testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dwyte\Projects\vdvs-backend\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\vortex-dwyte-voting-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123F0BB4-A5FA-43DE-8C19-5600D6D85DA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>lrn</t>
   </si>
@@ -93,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -404,11 +403,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -600,20 +599,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>310982184212</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>